<commit_message>
NDwr and SDwr update.
NDwr and SDwr update.
- added in scripts to remove "in-active" water rights.
</commit_message>
<xml_diff>
--- a/NorthDakota/WaterAllocation/NDwr_Allocation Schema Mapping to WaDE.xlsx
+++ b/NorthDakota/WaterAllocation/NDwr_Allocation Schema Mapping to WaDE.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rjame\Documents\WSWC Documents\MappingStatesDataToWaDE2.0\NorthDakota\WaterAllocation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7072AC98-3F2A-46D5-8902-11CB4A2ADEBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BD7D932-9D5F-440F-84A5-A3F6A31AC58F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="1692" windowWidth="23256" windowHeight="12456" tabRatio="714" activeTab="6" xr2:uid="{10FC1BAB-5472-410C-A2F0-85DCDF5389F8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" tabRatio="714" xr2:uid="{10FC1BAB-5472-410C-A2F0-85DCDF5389F8}"/>
   </bookViews>
   <sheets>
     <sheet name="Mapping Notes" sheetId="10" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1034" uniqueCount="300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1035" uniqueCount="301">
   <si>
     <t>Name</t>
   </si>
@@ -939,6 +939,9 @@
   </si>
   <si>
     <t>app_rate</t>
+  </si>
+  <si>
+    <t>For ND, we don't want water rights that are considered: Application In Processing, Cancelled, Deferred, Denied, Held In Abeyance, InActive, Pending Review Under Review, Void</t>
   </si>
 </sst>
 </file>
@@ -2304,8 +2307,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7154D4B-C952-456C-B506-1C3DB2041E3D}">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2357,6 +2360,11 @@
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>248</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>300</v>
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.3">
@@ -4609,8 +4617,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B91B1FF-D207-4871-B787-27544A9D3030}">
   <dimension ref="A1:P48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+    <sheetView topLeftCell="A43" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>